<commit_message>
2017-2024 list review page verified
</commit_message>
<xml_diff>
--- a/Results/DownloadListColored.xlsx
+++ b/Results/DownloadListColored.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo_q\Desktop\Working on\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312333D1-84DE-46C6-97C4-C326FD7459AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75613FA-A712-4513-9012-ED66AD8FA777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8970" yWindow="1430" windowWidth="28800" windowHeight="15060" xr2:uid="{64B2F72F-2EB2-4461-AFC4-CAED1B61A1FA}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{64B2F72F-2EB2-4461-AFC4-CAED1B61A1FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="1079">
   <si>
     <t>D_num</t>
   </si>
@@ -2418,6 +2418,861 @@
   </si>
   <si>
     <t>Need Investigate</t>
+  </si>
+  <si>
+    <t>Liberty Global PLC</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Liberty-Global-Reviews-E38776.htm</t>
+  </si>
+  <si>
+    <t>Array Biopharma Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Array-BioPharma-Reviews-E4648142.htm</t>
+  </si>
+  <si>
+    <t>Thorley Industries LLC</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/4moms-Reviews-E505096.htm</t>
+  </si>
+  <si>
+    <t>Physical Optics Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Mercury-Systems-Reviews-E4049.htm</t>
+  </si>
+  <si>
+    <t>IDT Corp</t>
+  </si>
+  <si>
+    <t>Cogint Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Fluent-Reviews-E825747.htm</t>
+  </si>
+  <si>
+    <t>RTI International</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/RTI-International-Reviews-E4480.htm</t>
+  </si>
+  <si>
+    <t>Stratasys Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Stratasys-Reviews-E3760.htm</t>
+  </si>
+  <si>
+    <t>Pentair plc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Pentair-Reviews-E1767.htm</t>
+  </si>
+  <si>
+    <t>Dover Corp</t>
+  </si>
+  <si>
+    <t>VC3 Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/VC3-Reviews-E394569.htm</t>
+  </si>
+  <si>
+    <t>Blackstone Group LP</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/The-Blackstone-Group-Reviews-E4022.htm</t>
+  </si>
+  <si>
+    <t>Wyndham Worldwide Corp to Destination</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Wyndham-Destinations-Reviews-E356401.htm</t>
+  </si>
+  <si>
+    <t>Wyndham Worldwide Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Wyndham-Hotels-and-Resorts-Reviews-E2310228.htm</t>
+  </si>
+  <si>
+    <t>Spirit Realty Capital Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Spirit-Realty-Capital-Reviews-E1844789.htm</t>
+  </si>
+  <si>
+    <t>Next Alt SARL</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Altice-USA-Reviews-E3190196.htm</t>
+  </si>
+  <si>
+    <t>DDR Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/DDR-Corp-Reviews-E2277.htm</t>
+  </si>
+  <si>
+    <t>LINN Energy Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Linn-Energy-Reviews-E38467.htm</t>
+  </si>
+  <si>
+    <t>Grupo Financiero Mercantil</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Banorte-Reviews-E8236.htm</t>
+  </si>
+  <si>
+    <t>Milliman Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Milliman-Reviews-E13873.htm</t>
+  </si>
+  <si>
+    <t>Inpixon</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Inpixon-Reviews-E1626192.htm</t>
+  </si>
+  <si>
+    <t>Klx Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/KLX-Energy-Services-Reviews-E1079236.htm</t>
+  </si>
+  <si>
+    <t>DHI Group Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/DHI-Group-Reviews-E1176264.htm</t>
+  </si>
+  <si>
+    <t>ServiceMaster Global Holdings Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/ServiceMaster-Brands-Reviews-E596.htm</t>
+  </si>
+  <si>
+    <t>Honeywell International Inc</t>
+  </si>
+  <si>
+    <t>Carolina Pad</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Carolina-Pad-Reviews-E2400339.htm</t>
+  </si>
+  <si>
+    <t>Trinity Industries Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Trinity-Industries-Reviews-E678.htm</t>
+  </si>
+  <si>
+    <t>Eqt Corp-Midstream Business</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/EQT-Corporation-Reviews-E233.htm</t>
+  </si>
+  <si>
+    <t>BGC Partners Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/BGC-Group-Reviews-E9862.htm</t>
+  </si>
+  <si>
+    <t>NETGEAR Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/NETGEAR-Reviews-E12666.htm</t>
+  </si>
+  <si>
+    <t>AECOM</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/AECOM-Reviews-E5632.htm</t>
+  </si>
+  <si>
+    <t>FMC Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/FMC-Reviews-E239.htm</t>
+  </si>
+  <si>
+    <t>Continental AG</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Continental-Reviews-E3768.htm</t>
+  </si>
+  <si>
+    <t>21st Century Fox Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/FOX-International-Channels-Reviews-E1018920.htm</t>
+  </si>
+  <si>
+    <t>Ironwood Pharmaceuticals Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Ironwood-Pharmaceuticals-Reviews-E262397.htm</t>
+  </si>
+  <si>
+    <t>DowDuPont Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Dow-Reviews-E207.htm</t>
+  </si>
+  <si>
+    <t>Onex Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Onex-Reviews-E6492.htm</t>
+  </si>
+  <si>
+    <t>Vertical Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Vertical-Screen-Reviews-E363989.htm</t>
+  </si>
+  <si>
+    <t>VF Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/VF-Reviews-E703.htm</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Corteva-Agriscience-Reviews-E2159858.htm</t>
+  </si>
+  <si>
+    <t>Thompson Street Capital Partners LP</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Thompson-Street-Capital-Partners-Reviews-E134472.htm</t>
+  </si>
+  <si>
+    <t>Whitepages Pro</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Whitepages-Reviews-E105846.htm</t>
+  </si>
+  <si>
+    <t>KAR Auction Services Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/OPENLANE-Reviews-E43271.htm</t>
+  </si>
+  <si>
+    <t>First Bankers Trustshares Inc, Quincy,Illinois</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/First-Banker-s-Trust-Reviews-E565480.htm</t>
+  </si>
+  <si>
+    <t>MYnd Analytics Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Emmaus-Life-Sciences-Reviews-E2246845.htm</t>
+  </si>
+  <si>
+    <t>Leader Bank NA</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Leader-Bank-Reviews-E348885.htm</t>
+  </si>
+  <si>
+    <t>Pickering Energy Partners LP</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Pickering-Energy-Partners-Reviews-E7422120.htm</t>
+  </si>
+  <si>
+    <t>Ensign Group Inc</t>
+  </si>
+  <si>
+    <t>Nuance Communications Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Nuance-Reviews-E5667.htm</t>
+  </si>
+  <si>
+    <t>Polo Digital Assets Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Poloniex-Reviews-E3202818.htm</t>
+  </si>
+  <si>
+    <t>Sverica Capital Management LP</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Sverica-Capital-Reviews-E2553217.htm</t>
+  </si>
+  <si>
+    <t>Taronis Fuels Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Taronis-Fuels-Reviews-E4517469.htm</t>
+  </si>
+  <si>
+    <t>Avant LLC</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Amount-Reviews-E3022487.htm</t>
+  </si>
+  <si>
+    <t>Cleartronic Inc</t>
+  </si>
+  <si>
+    <t>Brookfield Infrastructure Partners LP</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Brookfield-Reviews-E5824.htm</t>
+  </si>
+  <si>
+    <t>Chanticleer Holdings Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Chanticleer-Holdings-Reviews-E361270.htm</t>
+  </si>
+  <si>
+    <t>Arconic Inc</t>
+  </si>
+  <si>
+    <t>United Technologies Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/United-Technologies-Reviews-E697.htm</t>
+  </si>
+  <si>
+    <t>The Madison Square Garden Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Madison-Square-Garden-Reviews-E16146.htm</t>
+  </si>
+  <si>
+    <t>Sphero Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Sphero-Reviews-E1011752.htm</t>
+  </si>
+  <si>
+    <t>Greenpro Capital Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Greenpro-Capital-Group-Reviews-E1984795.htm</t>
+  </si>
+  <si>
+    <t>GreyLion Capital LP</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/GreyLion-Reviews-E9496697.htm</t>
+  </si>
+  <si>
+    <t>Kaufman Hall &amp; Associates LLC</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Kaufman-Hall-Reviews-E335498.htm</t>
+  </si>
+  <si>
+    <t>IAC/InterActiveCorp</t>
+  </si>
+  <si>
+    <t>Brookfield Asset Management Inc</t>
+  </si>
+  <si>
+    <t>Associated Capital Group Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Associated-Students-Inc-Reviews-E5829846.htm</t>
+  </si>
+  <si>
+    <t>HCI Equity Partners LLC</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/HCI-Equity-Partners-Reviews-E5371145.htm</t>
+  </si>
+  <si>
+    <t>American Outdoor Brands Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/American-Outdoor-Brands-Reviews-E1536306.htm</t>
+  </si>
+  <si>
+    <t>Intel Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Intel-Corporation-Reviews-E1519.htm</t>
+  </si>
+  <si>
+    <t>Folio Financial Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Folio-Financial-Inc-Reviews-E214427.htm</t>
+  </si>
+  <si>
+    <t>BFC Financial Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/BFC-Financial-Reviews-E23819.htm</t>
+  </si>
+  <si>
+    <t>LENSAR Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/LensAR-Reviews-E451185.htm</t>
+  </si>
+  <si>
+    <t>Fortive Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Fortive-Reviews-E1334602.htm</t>
+  </si>
+  <si>
+    <t>Searchlight Capital Partners LP</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Searchlight-Capital-Partners-Reviews-E1275302.htm</t>
+  </si>
+  <si>
+    <t>Myos Rens Technology Inc</t>
+  </si>
+  <si>
+    <t>GlaxoSmithKline PLC</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/GSK-Reviews-E3477.htm</t>
+  </si>
+  <si>
+    <t>SYNNEX Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/SYNNEX-Reviews-E12131.htm</t>
+  </si>
+  <si>
+    <t>Aaron's Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Aaron-s-Reviews-E1083.htm</t>
+  </si>
+  <si>
+    <t>Apartment Investment &amp; Management Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Aimco-Reviews-E24024.htm</t>
+  </si>
+  <si>
+    <t>Ameri Holdings Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Ameri100-A-TSP-Company-Reviews-E870394.htm</t>
+  </si>
+  <si>
+    <t>Gold Resource Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Platinum-Gold-Resource-Agency-Reviews-E5036743.htm</t>
+  </si>
+  <si>
+    <t>OncoImmune Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/OncoImmune-Reviews-E3220021.htm</t>
+  </si>
+  <si>
+    <t>Verint Systems Inc</t>
+  </si>
+  <si>
+    <t>Edwards Lifesciences Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Edwards-Lifesciences-Reviews-E11809.htm</t>
+  </si>
+  <si>
+    <t>Uber Technologies Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Uber-Reviews-E575263.htm</t>
+  </si>
+  <si>
+    <t>SinglePoint Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/SinglePoint-TX-Reviews-E7255719.htm</t>
+  </si>
+  <si>
+    <t>IAC/InteractiveCorp</t>
+  </si>
+  <si>
+    <t>Merck &amp; Co Inc</t>
+  </si>
+  <si>
+    <t>DTE Energy Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/DTE-Energy-Reviews-E199.htm</t>
+  </si>
+  <si>
+    <t>Silver Lake Partners LP</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Silver-Lake-Reviews-E11382.htm</t>
+  </si>
+  <si>
+    <t>L Brands Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/L-Brands-Reviews-E656.htm</t>
+  </si>
+  <si>
+    <t>XPO Logistics Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/XPO-Reviews-E615153.htm</t>
+  </si>
+  <si>
+    <t>International Paper Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/International-Paper-Reviews-E356.htm</t>
+  </si>
+  <si>
+    <t>J2 Global Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Ziff-Davis-Reviews-E6132150.htm</t>
+  </si>
+  <si>
+    <t>Arizona Lithium Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Arizona-Lithium-Reviews-E10664680.htm</t>
+  </si>
+  <si>
+    <t>Genie Energy Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Genie-Energy-Reviews-E1034949.htm</t>
+  </si>
+  <si>
+    <t>Dell Technologies Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Dell-Technologies-Reviews-E1327.htm</t>
+  </si>
+  <si>
+    <t>International Business Machines Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/IBM-Reviews-E354.htm</t>
+  </si>
+  <si>
+    <t>Beyond Cancer Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Living-Beyond-Breast-Cancer-Reviews-E1635365.htm</t>
+  </si>
+  <si>
+    <t>bluebird bio Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/bluebird-bio-Reviews-E729710.htm</t>
+  </si>
+  <si>
+    <t>Realty Income Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Realty-Income-Reviews-E3890.htm</t>
+  </si>
+  <si>
+    <t>Meredith Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Meredith-IA-Reviews-E6624707.htm</t>
+  </si>
+  <si>
+    <t>Vector Group Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Vector-Group-Reviews-E402.htm</t>
+  </si>
+  <si>
+    <t>PTC Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/PTC-Reviews-E1855.htm</t>
+  </si>
+  <si>
+    <t>Trutankless Inc</t>
+  </si>
+  <si>
+    <t>Neudesic LLC</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Neudesic-Reviews-E117212.htm</t>
+  </si>
+  <si>
+    <t>Constellation Energy Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Constellation-Energy-Reviews-E75.htm</t>
+  </si>
+  <si>
+    <t>Zimmer Biomet Holdings Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Zimmer-Biomet-Reviews-E1017414.htm</t>
+  </si>
+  <si>
+    <t>Becton Dickinson &amp; Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/BD-Reviews-E88.htm</t>
+  </si>
+  <si>
+    <t>Colfax Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Colfax-Reviews-E8723.htm</t>
+  </si>
+  <si>
+    <t>Pacific Coast Fruit Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Pacific-Coast-Fruit-Products-Reviews-E3221460.htm</t>
+  </si>
+  <si>
+    <t>Riordan Lewis &amp; Haden Equity Partners</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/RLH-Equity-Reviews-E1000750.htm</t>
+  </si>
+  <si>
+    <t>Vinco Ventures Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Vinco-Ventures-Reviews-E5811809.htm</t>
+  </si>
+  <si>
+    <t>Encompass Health Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Encompass-Health-Reviews-E1959649.htm</t>
+  </si>
+  <si>
+    <t>GSK plc</t>
+  </si>
+  <si>
+    <t>Fortress Transportation &amp; Infrastructure Investors LLC</t>
+  </si>
+  <si>
+    <t>Xperi Holding Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Xperi-Reviews-E1563777.htm</t>
+  </si>
+  <si>
+    <t>Biohaven Pharmaceutical Holding Co Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Biohaven-Pharmaceuticals-Reviews-E3054889.htm</t>
+  </si>
+  <si>
+    <t>Bluerock Residential Growth REIT Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Bluerock-Residential-Growth-Reviews-E5334287.htm</t>
+  </si>
+  <si>
+    <t>LGL Group Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/LGL-Group-Reviews-E927.htm</t>
+  </si>
+  <si>
+    <t>Fidelity National Financial Inc</t>
+  </si>
+  <si>
+    <t>Fortune Brands Home &amp; Security Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Fortune-Brands-Innovations-Reviews-E31.htm</t>
+  </si>
+  <si>
+    <t>General Electric Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/GE-Reviews-E277.htm</t>
+  </si>
+  <si>
+    <t>Jefferies Financial Group Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Jefferies-Reviews-E1546.htm</t>
+  </si>
+  <si>
+    <t>iStar Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/iStar-Reviews-E1262.htm</t>
+  </si>
+  <si>
+    <t>Crane Holdings Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Crane-Co-Reviews-E185.htm</t>
+  </si>
+  <si>
+    <t>Madison Square Garden Entertainment Corp</t>
+  </si>
+  <si>
+    <t>Curative Health Holdings Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Curative-Inc-Reviews-E3509458.htm</t>
+  </si>
+  <si>
+    <t>Petal Card Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Petal-Reviews-E1911245.htm</t>
+  </si>
+  <si>
+    <t>Meta Platforms Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Meta-Reviews-E40772.htm</t>
+  </si>
+  <si>
+    <t>Wisekey International Holding AG</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/WISeKey-Reviews-E34853.htm</t>
+  </si>
+  <si>
+    <t>Houston Natural Resources Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/ERM-Reviews-E13917.htm</t>
+  </si>
+  <si>
+    <t>MDU Resources Group Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/MDU-Resources-Reviews-E419.htm</t>
+  </si>
+  <si>
+    <t>Labcorp Holdings Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Labcorp-Reviews-E1679.htm</t>
+  </si>
+  <si>
+    <t>BorgWarner Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/BorgWarner-Reviews-E1652.htm</t>
+  </si>
+  <si>
+    <t>JS Global Lifestyle Co Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/JS-Global-Lifestyle-Reviews-E10325329.htm</t>
+  </si>
+  <si>
+    <t>Netography Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Netography-Reviews-E6894843.htm</t>
+  </si>
+  <si>
+    <t>Safe &amp; Green Holdings Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Safe-and-Green-Holdings-Reviews-E8372972.htm</t>
+  </si>
+  <si>
+    <t>Danaher Corp</t>
+  </si>
+  <si>
+    <t>Kellanova</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Kellanova-Reviews-E377.htm</t>
+  </si>
+  <si>
+    <t>Aramark Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Aramark-Reviews-E2716.htm</t>
+  </si>
+  <si>
+    <t>Utica Resource Ventures LLC</t>
+  </si>
+  <si>
+    <t>NCR Voyix Corp</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/NCR-Voyix-Reviews-E10016304.htm</t>
+  </si>
+  <si>
+    <t>WP Carey Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/W-P-Carey-Reviews-E7682.htm</t>
+  </si>
+  <si>
+    <t>Alkermes PLC</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Alkermes-Reviews-E1176.htm</t>
+  </si>
+  <si>
+    <t>Rough House Games Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Rough-House-Games-Reviews-E10120883.htm</t>
+  </si>
+  <si>
+    <t>Worthington Enterprises Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Worthington-Enterprises-Reviews-E2046.htm</t>
+  </si>
+  <si>
+    <t>Flex Ltd</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Flex-Reviews-E1036355.htm</t>
+  </si>
+  <si>
+    <t>Elda River Capital Management LLC</t>
+  </si>
+  <si>
+    <t>3M Co</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/3M-Reviews-E446.htm</t>
+  </si>
+  <si>
+    <t>Inhibrx Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Inhibrx-Reviews-E3237539.htm</t>
+  </si>
+  <si>
+    <t>Illumina Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Illumina-Reviews-E11671.htm</t>
+  </si>
+  <si>
+    <t>AFC Gamma Inc</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com/Reviews/Advanced-Flower-Capital-Gamma-Reviews-E5035901.htm</t>
   </si>
 </sst>
 </file>
@@ -2504,7 +3359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2521,6 +3376,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2836,10 +3696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056217F5-53D7-48E8-987C-B5C1231C4C2B}">
-  <dimension ref="A1:R202"/>
+  <dimension ref="A1:R361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="L151" sqref="L151:M151"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11327,9 +12187,3102 @@
         <v>8</v>
       </c>
     </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A203" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C203" s="18">
+        <v>42937</v>
+      </c>
+      <c r="D203" s="18">
+        <v>43102</v>
+      </c>
+      <c r="I203" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="L203" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="M203" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A204" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C204" s="18">
+        <v>43096</v>
+      </c>
+      <c r="D204" s="18">
+        <v>43104</v>
+      </c>
+      <c r="I204" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="L204" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="M204" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A205" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C205" s="18">
+        <v>42926</v>
+      </c>
+      <c r="D205" s="18">
+        <v>43154</v>
+      </c>
+      <c r="I205" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="L205" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="M205" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A206" s="17"/>
+      <c r="C206" s="18">
+        <v>43154</v>
+      </c>
+      <c r="D206" s="18">
+        <v>43154</v>
+      </c>
+      <c r="I206" s="6" t="s">
+        <v>800</v>
+      </c>
+      <c r="L206" s="6" t="s">
+        <v>801</v>
+      </c>
+      <c r="M206" s="6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A207" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C207" s="18">
+        <v>42817</v>
+      </c>
+      <c r="D207" s="18">
+        <v>43185</v>
+      </c>
+      <c r="I207" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="L207" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="M207" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A208" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C208" s="18">
+        <v>42985</v>
+      </c>
+      <c r="D208" s="18">
+        <v>43185</v>
+      </c>
+      <c r="I208" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="L208" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="M208" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A209" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C209" s="18">
+        <v>43186</v>
+      </c>
+      <c r="D209" s="18">
+        <v>43186</v>
+      </c>
+      <c r="I209" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="L209" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="M209" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A210" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C210" s="18">
+        <v>43193</v>
+      </c>
+      <c r="D210" s="18">
+        <v>43193</v>
+      </c>
+      <c r="I210" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="L210" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="M210" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A211" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C211" s="18">
+        <v>42864</v>
+      </c>
+      <c r="D211" s="18">
+        <v>43220</v>
+      </c>
+      <c r="I211" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="L211" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="M211" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A212" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C212" s="18">
+        <v>43076</v>
+      </c>
+      <c r="D212" s="18">
+        <v>43229</v>
+      </c>
+      <c r="I212" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="L212" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="M212" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A213" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C213" s="18">
+        <v>43231</v>
+      </c>
+      <c r="D213" s="18">
+        <v>43231</v>
+      </c>
+      <c r="I213" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="L213" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="M213" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A214" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C214" s="18">
+        <v>42753</v>
+      </c>
+      <c r="D214" s="18">
+        <v>43251</v>
+      </c>
+      <c r="I214" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="L214" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="M214" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A215" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C215" s="18">
+        <v>42968</v>
+      </c>
+      <c r="D215" s="18">
+        <v>43251</v>
+      </c>
+      <c r="I215" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="L215" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="M215" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A216" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C216" s="18">
+        <v>42949</v>
+      </c>
+      <c r="D216" s="18">
+        <v>43252</v>
+      </c>
+      <c r="I216" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="L216" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="M216" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A217" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C217" s="18">
+        <v>42950</v>
+      </c>
+      <c r="D217" s="18">
+        <v>43252</v>
+      </c>
+      <c r="I217" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="L217" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="M217" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A218" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C218" s="18">
+        <v>43108</v>
+      </c>
+      <c r="D218" s="18">
+        <v>43258</v>
+      </c>
+      <c r="I218" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="L218" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="M218" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A219" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C219" s="18">
+        <v>43083</v>
+      </c>
+      <c r="D219" s="18">
+        <v>43282</v>
+      </c>
+      <c r="I219" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="L219" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="M219" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A220" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C220" s="18">
+        <v>43208</v>
+      </c>
+      <c r="D220" s="18">
+        <v>43319</v>
+      </c>
+      <c r="I220" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="L220" s="16" t="s">
+        <v>827</v>
+      </c>
+      <c r="M220" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A221" s="17"/>
+      <c r="C221" s="18">
+        <v>43089</v>
+      </c>
+      <c r="D221" s="18">
+        <v>43322</v>
+      </c>
+      <c r="I221" s="13" t="s">
+        <v>828</v>
+      </c>
+      <c r="L221" s="13" t="s">
+        <v>829</v>
+      </c>
+      <c r="M221" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A222" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C222" s="18">
+        <v>43332</v>
+      </c>
+      <c r="D222" s="18">
+        <v>43332</v>
+      </c>
+      <c r="I222" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="L222" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="M222" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A223" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C223" s="18">
+        <v>43207</v>
+      </c>
+      <c r="D223" s="18">
+        <v>43347</v>
+      </c>
+      <c r="I223" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="L223" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="M223" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A224" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C224" s="18">
+        <v>43221</v>
+      </c>
+      <c r="D224" s="18">
+        <v>43357</v>
+      </c>
+      <c r="I224" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="L224" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="M224" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A225" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C225" s="18">
+        <v>43360</v>
+      </c>
+      <c r="D225" s="18">
+        <v>43360</v>
+      </c>
+      <c r="I225" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="L225" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="M225" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A226" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C226" s="18">
+        <v>42942</v>
+      </c>
+      <c r="D226" s="18">
+        <v>43374</v>
+      </c>
+      <c r="I226" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="L226" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="M226" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A227" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C227" s="18">
+        <v>43018</v>
+      </c>
+      <c r="D227" s="18">
+        <v>43374</v>
+      </c>
+      <c r="I227" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="L227" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="M227" s="2">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A228" s="17"/>
+      <c r="C228" s="18">
+        <v>43053</v>
+      </c>
+      <c r="D228" s="18">
+        <v>43384</v>
+      </c>
+      <c r="I228" s="13" t="s">
+        <v>841</v>
+      </c>
+      <c r="L228" s="13" t="s">
+        <v>842</v>
+      </c>
+      <c r="M228" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A229" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C229" s="18">
+        <v>43018</v>
+      </c>
+      <c r="D229" s="18">
+        <v>43402</v>
+      </c>
+      <c r="I229" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="L229" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="M229" s="2">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A230" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C230" s="18">
+        <v>43081</v>
+      </c>
+      <c r="D230" s="18">
+        <v>43405</v>
+      </c>
+      <c r="I230" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="L230" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="M230" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A231" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C231" s="18">
+        <v>43152</v>
+      </c>
+      <c r="D231" s="18">
+        <v>43416</v>
+      </c>
+      <c r="I231" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="L231" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="M231" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A232" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C232" s="18">
+        <v>43140</v>
+      </c>
+      <c r="D232" s="18">
+        <v>43434</v>
+      </c>
+      <c r="I232" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="L232" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="M232" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A233" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C233" s="18">
+        <v>43433</v>
+      </c>
+      <c r="D233" s="18">
+        <v>43465</v>
+      </c>
+      <c r="I233" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="L233" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="M233" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A234" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C234" s="18">
+        <v>43493</v>
+      </c>
+      <c r="D234" s="18">
+        <v>43493</v>
+      </c>
+      <c r="I234" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="L234" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="M234" s="2">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A235" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C235" s="18">
+        <v>43507</v>
+      </c>
+      <c r="D235" s="18">
+        <v>43525</v>
+      </c>
+      <c r="I235" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="L235" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="M235" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A236" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C236" s="18">
+        <v>43536</v>
+      </c>
+      <c r="D236" s="18">
+        <v>43536</v>
+      </c>
+      <c r="I236" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="L236" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="M236" s="2">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A237" s="17"/>
+      <c r="C237" s="18">
+        <v>43083</v>
+      </c>
+      <c r="D237" s="18">
+        <v>43543</v>
+      </c>
+      <c r="I237" s="6" t="s">
+        <v>857</v>
+      </c>
+      <c r="L237" s="6" t="s">
+        <v>858</v>
+      </c>
+      <c r="M237" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A238" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C238" s="18">
+        <v>43221</v>
+      </c>
+      <c r="D238" s="18">
+        <v>43556</v>
+      </c>
+      <c r="I238" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="L238" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="M238" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A239" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C239" s="18">
+        <v>43349</v>
+      </c>
+      <c r="D239" s="18">
+        <v>43556</v>
+      </c>
+      <c r="I239" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L239" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="M239" s="2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A240" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C240" s="18">
+        <v>43556</v>
+      </c>
+      <c r="D240" s="18">
+        <v>43556</v>
+      </c>
+      <c r="I240" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="L240" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="M240" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A241" s="17"/>
+      <c r="C241" s="18">
+        <v>43493</v>
+      </c>
+      <c r="D241" s="18">
+        <v>43557</v>
+      </c>
+      <c r="I241" s="13" t="s">
+        <v>865</v>
+      </c>
+      <c r="L241" s="13" t="s">
+        <v>866</v>
+      </c>
+      <c r="M241" s="13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A242" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C242" s="18">
+        <v>43325</v>
+      </c>
+      <c r="D242" s="18">
+        <v>43608</v>
+      </c>
+      <c r="I242" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="L242" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="M242" s="2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A243" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C243" s="18">
+        <v>43349</v>
+      </c>
+      <c r="D243" s="18">
+        <v>43617</v>
+      </c>
+      <c r="I243" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L243" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="M243" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A244" s="17"/>
+      <c r="C244" s="18">
+        <v>43622</v>
+      </c>
+      <c r="D244" s="18">
+        <v>43622</v>
+      </c>
+      <c r="I244" s="13" t="s">
+        <v>870</v>
+      </c>
+      <c r="L244" s="13" t="s">
+        <v>871</v>
+      </c>
+      <c r="M244" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A245" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C245" s="18">
+        <v>43628</v>
+      </c>
+      <c r="D245" s="18">
+        <v>43628</v>
+      </c>
+      <c r="I245" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="L245" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="M245" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A246" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C246" s="18">
+        <v>43158</v>
+      </c>
+      <c r="D246" s="18">
+        <v>43644</v>
+      </c>
+      <c r="I246" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="L246" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="M246" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A247" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C247" s="18">
+        <v>43621</v>
+      </c>
+      <c r="D247" s="18">
+        <v>43647</v>
+      </c>
+      <c r="I247" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="L247" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="M247" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A248" s="17"/>
+      <c r="C248" s="18">
+        <v>43472</v>
+      </c>
+      <c r="D248" s="18">
+        <v>43663</v>
+      </c>
+      <c r="I248" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="L248" s="6" t="s">
+        <v>879</v>
+      </c>
+      <c r="M248" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A249" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C249" s="18">
+        <v>43692</v>
+      </c>
+      <c r="D249" s="18">
+        <v>43692</v>
+      </c>
+      <c r="I249" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="L249" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="M249" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A250" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C250" s="18">
+        <v>43714</v>
+      </c>
+      <c r="D250" s="18">
+        <v>43714</v>
+      </c>
+      <c r="I250" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="L250" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="M250" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A251" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C251" s="18">
+        <v>43591</v>
+      </c>
+      <c r="D251" s="18">
+        <v>43739</v>
+      </c>
+      <c r="I251" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="L251" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="M251" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A252" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C252" s="18">
+        <v>43423</v>
+      </c>
+      <c r="D252" s="18">
+        <v>43740</v>
+      </c>
+      <c r="I252" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="L252" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="M252" s="2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A253" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C253" s="18">
+        <v>43756</v>
+      </c>
+      <c r="D253" s="18">
+        <v>43756</v>
+      </c>
+      <c r="I253" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="L253" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="M253" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A254" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C254" s="18">
+        <v>43760</v>
+      </c>
+      <c r="D254" s="18">
+        <v>43760</v>
+      </c>
+      <c r="I254" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="L254" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="M254" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A255" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C255" s="18">
+        <v>43661</v>
+      </c>
+      <c r="D255" s="18">
+        <v>43798</v>
+      </c>
+      <c r="I255" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="L255" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="M255" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A256" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C256" s="18">
+        <v>43866</v>
+      </c>
+      <c r="D256" s="18">
+        <v>43866</v>
+      </c>
+      <c r="I256" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="L256" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="M256" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A257" s="17"/>
+      <c r="C257" s="18">
+        <v>43377</v>
+      </c>
+      <c r="D257" s="18">
+        <v>43875</v>
+      </c>
+      <c r="I257" s="13" t="s">
+        <v>895</v>
+      </c>
+      <c r="L257" s="13"/>
+      <c r="M257" s="13"/>
+    </row>
+    <row r="258" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A258" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C258" s="18">
+        <v>43733</v>
+      </c>
+      <c r="D258" s="18">
+        <v>43921</v>
+      </c>
+      <c r="I258" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="L258" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="M258" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A259" s="17"/>
+      <c r="C259" s="18">
+        <v>43748</v>
+      </c>
+      <c r="D259" s="18">
+        <v>43922</v>
+      </c>
+      <c r="I259" s="13" t="s">
+        <v>898</v>
+      </c>
+      <c r="L259" s="13" t="s">
+        <v>899</v>
+      </c>
+      <c r="M259" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A260" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C260" s="18">
+        <v>43502</v>
+      </c>
+      <c r="D260" s="18">
+        <v>43922</v>
+      </c>
+      <c r="I260" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="L260" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="M260" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A261" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C261" s="18">
+        <v>43430</v>
+      </c>
+      <c r="D261" s="18">
+        <v>43924</v>
+      </c>
+      <c r="I261" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="L261" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="M261" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A262" s="17"/>
+      <c r="C262" s="18">
+        <v>43430</v>
+      </c>
+      <c r="D262" s="18">
+        <v>43924</v>
+      </c>
+      <c r="I262" t="s">
+        <v>901</v>
+      </c>
+      <c r="L262" t="s">
+        <v>902</v>
+      </c>
+      <c r="M262">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A263" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C263" s="18">
+        <v>43278</v>
+      </c>
+      <c r="D263" s="18">
+        <v>43941</v>
+      </c>
+      <c r="I263" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="L263" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="M263" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A264" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C264" s="18">
+        <v>43971</v>
+      </c>
+      <c r="D264" s="18">
+        <v>43971</v>
+      </c>
+      <c r="I264" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="L264" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="M264" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A265" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C265" s="18">
+        <v>43984</v>
+      </c>
+      <c r="D265" s="18">
+        <v>43984</v>
+      </c>
+      <c r="I265" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="L265" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="M265" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A266" s="17"/>
+      <c r="C266" s="18">
+        <v>43998</v>
+      </c>
+      <c r="D266" s="18">
+        <v>43998</v>
+      </c>
+      <c r="I266" s="13" t="s">
+        <v>909</v>
+      </c>
+      <c r="L266" s="13" t="s">
+        <v>910</v>
+      </c>
+      <c r="M266" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A267" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C267" s="18">
+        <v>44007</v>
+      </c>
+      <c r="D267" s="18">
+        <v>44007</v>
+      </c>
+      <c r="I267" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="L267" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="M267" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A268" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C268" s="18">
+        <v>43684</v>
+      </c>
+      <c r="D268" s="18">
+        <v>44012</v>
+      </c>
+      <c r="I268" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="L268" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="M268" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A269" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C269" s="18">
+        <v>43780</v>
+      </c>
+      <c r="D269" s="18">
+        <v>44042</v>
+      </c>
+      <c r="I269" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="L269" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="M269" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A270" s="17"/>
+      <c r="C270" s="18">
+        <v>43906</v>
+      </c>
+      <c r="D270" s="18">
+        <v>44048</v>
+      </c>
+      <c r="I270" s="13" t="s">
+        <v>915</v>
+      </c>
+      <c r="L270" s="13" t="s">
+        <v>916</v>
+      </c>
+      <c r="M270" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A271" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C271" s="18">
+        <v>44039</v>
+      </c>
+      <c r="D271" s="18">
+        <v>44050</v>
+      </c>
+      <c r="I271" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="L271" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="M271" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A272" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C272" s="18">
+        <v>43782</v>
+      </c>
+      <c r="D272" s="18">
+        <v>44067</v>
+      </c>
+      <c r="I272" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="L272" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="M272" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A273" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C273" s="18">
+        <v>44093</v>
+      </c>
+      <c r="D273" s="18">
+        <v>44093</v>
+      </c>
+      <c r="I273" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="L273" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="M273" s="2">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A274" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C274" s="18">
+        <v>44092</v>
+      </c>
+      <c r="D274" s="18">
+        <v>44095</v>
+      </c>
+      <c r="I274" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="L274" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="M274" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A275" s="17"/>
+      <c r="C275" s="18">
+        <v>43999</v>
+      </c>
+      <c r="D275" s="18">
+        <v>44104</v>
+      </c>
+      <c r="I275" s="13" t="s">
+        <v>925</v>
+      </c>
+      <c r="L275" s="13" t="s">
+        <v>926</v>
+      </c>
+      <c r="M275" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A276" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C276" s="18">
+        <v>44069</v>
+      </c>
+      <c r="D276" s="18">
+        <v>44106</v>
+      </c>
+      <c r="I276" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="L276" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="M276" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A277" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C277" s="18">
+        <v>43712</v>
+      </c>
+      <c r="D277" s="18">
+        <v>44113</v>
+      </c>
+      <c r="I277" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="L277" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="M277" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A278" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C278" s="18">
+        <v>44125</v>
+      </c>
+      <c r="D278" s="18">
+        <v>44125</v>
+      </c>
+      <c r="I278" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="L278" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="M278" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A279" s="17"/>
+      <c r="C279" s="18">
+        <v>44012</v>
+      </c>
+      <c r="D279" s="18">
+        <v>44151</v>
+      </c>
+      <c r="I279" s="13" t="s">
+        <v>933</v>
+      </c>
+      <c r="L279" s="13"/>
+      <c r="M279" s="13"/>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A280" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C280" s="18">
+        <v>44154</v>
+      </c>
+      <c r="D280" s="18">
+        <v>44154</v>
+      </c>
+      <c r="I280" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="L280" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="M280" s="2">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A281" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C281" s="18">
+        <v>43839</v>
+      </c>
+      <c r="D281" s="18">
+        <v>44166</v>
+      </c>
+      <c r="I281" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="L281" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="M281" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A282" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C282" s="18">
+        <v>44041</v>
+      </c>
+      <c r="D282" s="18">
+        <v>44166</v>
+      </c>
+      <c r="I282" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="L282" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="M282" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A283" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C283" s="18">
+        <v>44088</v>
+      </c>
+      <c r="D283" s="18">
+        <v>44180</v>
+      </c>
+      <c r="I283" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="L283" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="M283" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A284" s="17"/>
+      <c r="C284" s="18">
+        <v>43843</v>
+      </c>
+      <c r="D284" s="18">
+        <v>44196</v>
+      </c>
+      <c r="I284" s="13" t="s">
+        <v>942</v>
+      </c>
+      <c r="L284" s="13" t="s">
+        <v>943</v>
+      </c>
+      <c r="M284" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A285" s="17"/>
+      <c r="C285" s="18">
+        <v>44109</v>
+      </c>
+      <c r="D285" s="18">
+        <v>44196</v>
+      </c>
+      <c r="I285" s="13" t="s">
+        <v>944</v>
+      </c>
+      <c r="L285" s="13" t="s">
+        <v>945</v>
+      </c>
+      <c r="M285" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A286" s="17"/>
+      <c r="C286" s="18">
+        <v>44158</v>
+      </c>
+      <c r="D286" s="18">
+        <v>44196</v>
+      </c>
+      <c r="I286" s="13" t="s">
+        <v>946</v>
+      </c>
+      <c r="L286" s="13" t="s">
+        <v>947</v>
+      </c>
+      <c r="M286" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A287" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C287" s="18">
+        <v>43803</v>
+      </c>
+      <c r="D287" s="18">
+        <v>44228</v>
+      </c>
+      <c r="I287" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="L287" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="M287" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A288" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C288" s="18">
+        <v>44237</v>
+      </c>
+      <c r="D288" s="18">
+        <v>44237</v>
+      </c>
+      <c r="I288" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="L288" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="M288" s="2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A289" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C289" s="18">
+        <v>44257</v>
+      </c>
+      <c r="D289" s="18">
+        <v>44257</v>
+      </c>
+      <c r="I289" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="L289" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="M289" s="2">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A290" s="17"/>
+      <c r="C290" s="18">
+        <v>44281</v>
+      </c>
+      <c r="D290" s="18">
+        <v>44293</v>
+      </c>
+      <c r="I290" s="13" t="s">
+        <v>953</v>
+      </c>
+      <c r="L290" s="13" t="s">
+        <v>954</v>
+      </c>
+      <c r="M290" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A291" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C291" s="18">
+        <v>44187</v>
+      </c>
+      <c r="D291" s="18">
+        <v>44341</v>
+      </c>
+      <c r="I291" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="L291" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="M291" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A292" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C292" s="18">
+        <v>43866</v>
+      </c>
+      <c r="D292" s="18">
+        <v>44349</v>
+      </c>
+      <c r="I292" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="L292" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M292" s="2">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="293" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A293" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C293" s="18">
+        <v>44131</v>
+      </c>
+      <c r="D293" s="18">
+        <v>44378</v>
+      </c>
+      <c r="I293" s="2" t="s">
+        <v>957</v>
+      </c>
+      <c r="L293" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="M293" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="294" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A294" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C294" s="18">
+        <v>44049</v>
+      </c>
+      <c r="D294" s="18">
+        <v>44396</v>
+      </c>
+      <c r="I294" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="L294" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="M294" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A295" s="17"/>
+      <c r="C295" s="18">
+        <v>43955</v>
+      </c>
+      <c r="D295" s="18">
+        <v>44410</v>
+      </c>
+      <c r="I295" s="13" t="s">
+        <v>961</v>
+      </c>
+      <c r="L295" s="13" t="s">
+        <v>962</v>
+      </c>
+      <c r="M295" s="13">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A296" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C296" s="18">
+        <v>44167</v>
+      </c>
+      <c r="D296" s="18">
+        <v>44410</v>
+      </c>
+      <c r="I296" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="L296" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="M296" s="2">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A297" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C297" s="18">
+        <v>43881</v>
+      </c>
+      <c r="D297" s="18">
+        <v>44411</v>
+      </c>
+      <c r="I297" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="L297" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="M297" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A298" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C298" s="18">
+        <v>44168</v>
+      </c>
+      <c r="D298" s="18">
+        <v>44470</v>
+      </c>
+      <c r="I298" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="L298" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="M298" s="2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="299" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A299" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C299" s="18">
+        <v>44305</v>
+      </c>
+      <c r="D299" s="18">
+        <v>44476</v>
+      </c>
+      <c r="I299" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="L299" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="M299" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A300" s="17"/>
+      <c r="C300" s="18">
+        <v>44350</v>
+      </c>
+      <c r="D300" s="18">
+        <v>44477</v>
+      </c>
+      <c r="I300" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="L300" s="13" t="s">
+        <v>970</v>
+      </c>
+      <c r="M300" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A301" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C301" s="18">
+        <v>44483</v>
+      </c>
+      <c r="D301" s="18">
+        <v>44483</v>
+      </c>
+      <c r="I301" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="L301" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="M301" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A302" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C302" s="18">
+        <v>44027</v>
+      </c>
+      <c r="D302" s="18">
+        <v>44501</v>
+      </c>
+      <c r="I302" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="L302" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="M302" s="2">
+        <v>3540</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A303" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C303" s="18">
+        <v>44112</v>
+      </c>
+      <c r="D303" s="18">
+        <v>44503</v>
+      </c>
+      <c r="I303" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="L303" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="M303" s="2">
+        <v>10430</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A304" s="17"/>
+      <c r="C304" s="18">
+        <v>44504</v>
+      </c>
+      <c r="D304" s="18">
+        <v>44504</v>
+      </c>
+      <c r="I304" s="13" t="s">
+        <v>977</v>
+      </c>
+      <c r="L304" s="13" t="s">
+        <v>978</v>
+      </c>
+      <c r="M304" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A305" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C305" s="18">
+        <v>44207</v>
+      </c>
+      <c r="D305" s="18">
+        <v>44505</v>
+      </c>
+      <c r="I305" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="L305" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="M305" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A306" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C306" s="18">
+        <v>44315</v>
+      </c>
+      <c r="D306" s="18">
+        <v>44515</v>
+      </c>
+      <c r="I306" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="L306" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="M306" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A307" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C307" s="18">
+        <v>44319</v>
+      </c>
+      <c r="D307" s="18">
+        <v>44531</v>
+      </c>
+      <c r="I307" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="L307" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="M307" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A308" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C308" s="18">
+        <v>44508</v>
+      </c>
+      <c r="D308" s="18">
+        <v>44560</v>
+      </c>
+      <c r="I308" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="L308" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="M308" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A309" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C309" s="18">
+        <v>44573</v>
+      </c>
+      <c r="D309" s="18">
+        <v>44573</v>
+      </c>
+      <c r="I309" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="L309" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="M309" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="310" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A310" s="17"/>
+      <c r="C310" s="18">
+        <v>44484</v>
+      </c>
+      <c r="D310" s="18">
+        <v>44582</v>
+      </c>
+      <c r="I310" s="13" t="s">
+        <v>989</v>
+      </c>
+      <c r="L310" s="13"/>
+      <c r="M310" s="13"/>
+    </row>
+    <row r="311" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A311" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C311" s="18">
+        <v>44587</v>
+      </c>
+      <c r="D311" s="18">
+        <v>44587</v>
+      </c>
+      <c r="I311" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="L311" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="M311" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="312" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A312" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C312" s="18">
+        <v>44251</v>
+      </c>
+      <c r="D312" s="18">
+        <v>44593</v>
+      </c>
+      <c r="I312" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="L312" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="M312" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A313" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C313" s="18">
+        <v>44232</v>
+      </c>
+      <c r="D313" s="18">
+        <v>44621</v>
+      </c>
+      <c r="I313" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="L313" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="M313" s="2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A314" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C314" s="18">
+        <v>44410</v>
+      </c>
+      <c r="D314" s="18">
+        <v>44635</v>
+      </c>
+      <c r="I314" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="L314" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="M314" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A315" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C315" s="18">
+        <v>44322</v>
+      </c>
+      <c r="D315" s="18">
+        <v>44652</v>
+      </c>
+      <c r="I315" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="L315" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="M315" s="2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A316" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C316" s="18">
+        <v>44259</v>
+      </c>
+      <c r="D316" s="18">
+        <v>44655</v>
+      </c>
+      <c r="I316" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="L316" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="M316" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A317" s="17"/>
+      <c r="C317" s="18">
+        <v>44671</v>
+      </c>
+      <c r="D317" s="18">
+        <v>44671</v>
+      </c>
+      <c r="I317" s="13" t="s">
+        <v>1000</v>
+      </c>
+      <c r="L317" s="13" t="s">
+        <v>1001</v>
+      </c>
+      <c r="M317" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A318" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C318" s="18">
+        <v>44677</v>
+      </c>
+      <c r="D318" s="18">
+        <v>44677</v>
+      </c>
+      <c r="I318" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L318" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="M318" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A319" s="17"/>
+      <c r="C319" s="18">
+        <v>44508</v>
+      </c>
+      <c r="D319" s="18">
+        <v>44742</v>
+      </c>
+      <c r="I319" s="13" t="s">
+        <v>1004</v>
+      </c>
+      <c r="L319" s="13" t="s">
+        <v>1005</v>
+      </c>
+      <c r="M319" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A320" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C320" s="18">
+        <v>44580</v>
+      </c>
+      <c r="D320" s="18">
+        <v>44743</v>
+      </c>
+      <c r="I320" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="L320" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="M320" s="2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="321" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A321" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C321" s="18">
+        <v>44230</v>
+      </c>
+      <c r="D321" s="18">
+        <v>44760</v>
+      </c>
+      <c r="I321" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="L321" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="M321" s="2">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="322" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A322" s="17"/>
+      <c r="C322" s="18">
+        <v>44550</v>
+      </c>
+      <c r="D322" s="18">
+        <v>44774</v>
+      </c>
+      <c r="I322" s="13" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L322" s="13"/>
+      <c r="M322" s="13"/>
+    </row>
+    <row r="323" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A323" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C323" s="18">
+        <v>43594</v>
+      </c>
+      <c r="D323" s="18">
+        <v>44837</v>
+      </c>
+      <c r="I323" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="L323" s="2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="M323" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="324" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A324" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C324" s="18">
+        <v>44822</v>
+      </c>
+      <c r="D324" s="18">
+        <v>44837</v>
+      </c>
+      <c r="I324" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="L324" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="M324" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="325" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A325" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C325" s="18">
+        <v>44550</v>
+      </c>
+      <c r="D325" s="18">
+        <v>44840</v>
+      </c>
+      <c r="I325" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="L325" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="M325" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A326" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C326" s="18">
+        <v>44420</v>
+      </c>
+      <c r="D326" s="18">
+        <v>44841</v>
+      </c>
+      <c r="I326" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L326" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="M326" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A327" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C327" s="18">
+        <v>44628</v>
+      </c>
+      <c r="D327" s="18">
+        <v>44866</v>
+      </c>
+      <c r="I327" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="L327" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="M327" s="2">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="328" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A328" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C328" s="18">
+        <v>44636</v>
+      </c>
+      <c r="D328" s="18">
+        <v>44896</v>
+      </c>
+      <c r="I328" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="L328" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="M328" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="329" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A329" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C329" s="18">
+        <v>44679</v>
+      </c>
+      <c r="D329" s="18">
+        <v>44909</v>
+      </c>
+      <c r="I329" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="L329" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M329" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="330" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A330" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C330" s="18">
+        <v>44509</v>
+      </c>
+      <c r="D330" s="18">
+        <v>44929</v>
+      </c>
+      <c r="I330" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L330" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="M330" s="2">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="331" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A331" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C331" s="18">
+        <v>44761</v>
+      </c>
+      <c r="D331" s="18">
+        <v>44943</v>
+      </c>
+      <c r="I331" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L331" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="M331" s="2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="332" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A332" s="17"/>
+      <c r="C332" s="18">
+        <v>44784</v>
+      </c>
+      <c r="D332" s="18">
+        <v>45016</v>
+      </c>
+      <c r="I332" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="L332" s="6" t="s">
+        <v>1026</v>
+      </c>
+      <c r="M332" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="333" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A333" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C333" s="18">
+        <v>44650</v>
+      </c>
+      <c r="D333" s="18">
+        <v>45019</v>
+      </c>
+      <c r="I333" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="L333" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="M333" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="334" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A334" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C334" s="18">
+        <v>44860</v>
+      </c>
+      <c r="D334" s="18">
+        <v>45036</v>
+      </c>
+      <c r="I334" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L334" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="M334" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="335" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A335" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C335" s="18">
+        <v>45040</v>
+      </c>
+      <c r="D335" s="18">
+        <v>45040</v>
+      </c>
+      <c r="I335" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="L335" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="M335" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="336" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A336" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C336" s="18">
+        <v>45056</v>
+      </c>
+      <c r="D336" s="18">
+        <v>45056</v>
+      </c>
+      <c r="I336" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="L336" s="2" t="s">
+        <v>1033</v>
+      </c>
+      <c r="M336" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A337" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C337" s="18">
+        <v>45062</v>
+      </c>
+      <c r="D337" s="18">
+        <v>45062</v>
+      </c>
+      <c r="I337" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="L337" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="M337" s="2">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A338" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C338" s="18">
+        <v>44970</v>
+      </c>
+      <c r="D338" s="18">
+        <v>45068</v>
+      </c>
+      <c r="I338" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="L338" s="2" t="s">
+        <v>1037</v>
+      </c>
+      <c r="M338" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A339" s="17"/>
+      <c r="C339" s="18">
+        <v>44748</v>
+      </c>
+      <c r="D339" s="18">
+        <v>45072</v>
+      </c>
+      <c r="I339" s="13" t="s">
+        <v>1038</v>
+      </c>
+      <c r="L339" s="13" t="s">
+        <v>1039</v>
+      </c>
+      <c r="M339" s="13">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A340" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C340" s="18">
+        <v>44777</v>
+      </c>
+      <c r="D340" s="18">
+        <v>45078</v>
+      </c>
+      <c r="I340" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L340" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="M340" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A341" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C341" s="18">
+        <v>44770</v>
+      </c>
+      <c r="D341" s="18">
+        <v>45110</v>
+      </c>
+      <c r="I341" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="L341" s="2" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M341" s="2">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A342" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C342" s="18">
+        <v>44901</v>
+      </c>
+      <c r="D342" s="18">
+        <v>45110</v>
+      </c>
+      <c r="I342" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L342" s="2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="M342" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A343" s="17"/>
+      <c r="C343" s="18">
+        <v>44980</v>
+      </c>
+      <c r="D343" s="18">
+        <v>45138</v>
+      </c>
+      <c r="I343" s="13" t="s">
+        <v>1046</v>
+      </c>
+      <c r="L343" s="13" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M343" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A344" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C344" s="18">
+        <v>45181</v>
+      </c>
+      <c r="D344" s="18">
+        <v>45181</v>
+      </c>
+      <c r="I344" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="L344" s="2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="M344" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A345" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C345" s="18">
+        <v>44918</v>
+      </c>
+      <c r="D345" s="18">
+        <v>45197</v>
+      </c>
+      <c r="I345" s="2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="L345" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="M345" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A346" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C346" s="18">
+        <v>44818</v>
+      </c>
+      <c r="D346" s="18">
+        <v>45199</v>
+      </c>
+      <c r="I346" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="L346" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="M346" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A347" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C347" s="18">
+        <v>44733</v>
+      </c>
+      <c r="D347" s="18">
+        <v>45201</v>
+      </c>
+      <c r="I347" s="2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="L347" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="M347" s="2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A348" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C348" s="18">
+        <v>44691</v>
+      </c>
+      <c r="D348" s="18">
+        <v>45201</v>
+      </c>
+      <c r="I348" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="L348" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="M348" s="2">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A349" s="17"/>
+      <c r="C349" s="18">
+        <v>45203</v>
+      </c>
+      <c r="D349" s="18">
+        <v>45203</v>
+      </c>
+      <c r="I349" s="13" t="s">
+        <v>1057</v>
+      </c>
+      <c r="L349" s="13"/>
+      <c r="M349" s="13"/>
+    </row>
+    <row r="350" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A350" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C350" s="18">
+        <v>44819</v>
+      </c>
+      <c r="D350" s="18">
+        <v>45215</v>
+      </c>
+      <c r="I350" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="L350" s="2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="M350" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A351" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C351" s="18">
+        <v>45189</v>
+      </c>
+      <c r="D351" s="18">
+        <v>45231</v>
+      </c>
+      <c r="I351" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="L351" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="M351" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A352" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C352" s="18">
+        <v>44867</v>
+      </c>
+      <c r="D352" s="18">
+        <v>45245</v>
+      </c>
+      <c r="I352" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L352" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="M352" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A353" s="17"/>
+      <c r="C353" s="18">
+        <v>45251</v>
+      </c>
+      <c r="D353" s="18">
+        <v>45251</v>
+      </c>
+      <c r="I353" s="13" t="s">
+        <v>1064</v>
+      </c>
+      <c r="L353" s="13" t="s">
+        <v>1065</v>
+      </c>
+      <c r="M353" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A354" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C354" s="18">
+        <v>44833</v>
+      </c>
+      <c r="D354" s="18">
+        <v>45261</v>
+      </c>
+      <c r="I354" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="L354" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="M354" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A355" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C355" s="18">
+        <v>44958</v>
+      </c>
+      <c r="D355" s="18">
+        <v>45293</v>
+      </c>
+      <c r="I355" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="L355" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="M355" s="2">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A356" s="17"/>
+      <c r="C356" s="18">
+        <v>45351</v>
+      </c>
+      <c r="D356" s="18">
+        <v>45351</v>
+      </c>
+      <c r="I356" s="13" t="s">
+        <v>1070</v>
+      </c>
+      <c r="L356" s="13"/>
+      <c r="M356" s="13"/>
+    </row>
+    <row r="357" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A357" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C357" s="18">
+        <v>44768</v>
+      </c>
+      <c r="D357" s="18">
+        <v>45383</v>
+      </c>
+      <c r="I357" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="L357" s="2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="M357" s="2">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A358" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C358" s="18">
+        <v>44509</v>
+      </c>
+      <c r="D358" s="18">
+        <v>45384</v>
+      </c>
+      <c r="I358" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L358" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="M358" s="2">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A359" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C359" s="18">
+        <v>45314</v>
+      </c>
+      <c r="D359" s="18">
+        <v>45442</v>
+      </c>
+      <c r="I359" s="2" t="s">
+        <v>1073</v>
+      </c>
+      <c r="L359" s="2" t="s">
+        <v>1074</v>
+      </c>
+      <c r="M359" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A360" s="17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C360" s="18">
+        <v>45446</v>
+      </c>
+      <c r="D360" s="18">
+        <v>45467</v>
+      </c>
+      <c r="I360" s="2" t="s">
+        <v>1075</v>
+      </c>
+      <c r="L360" s="2" t="s">
+        <v>1076</v>
+      </c>
+      <c r="M360" s="2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A361" s="17"/>
+      <c r="C361" s="18">
+        <v>45344</v>
+      </c>
+      <c r="D361" s="18">
+        <v>45482</v>
+      </c>
+      <c r="I361" s="13" t="s">
+        <v>1077</v>
+      </c>
+      <c r="L361" s="13" t="s">
+        <v>1078</v>
+      </c>
+      <c r="M361" s="13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L141" r:id="rId1" xr:uid="{1E14D960-A1F2-4DCC-A8E1-E88D7CF69EB3}"/>
+    <hyperlink ref="L220" r:id="rId2" xr:uid="{226DA921-7870-4847-84AA-4001323BD4AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>